<commit_message>
Modifications to lists and added training set
</commit_message>
<xml_diff>
--- a/trainingSets/explicit.xlsx
+++ b/trainingSets/explicit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manukastratta/Box Sync/STANFORD/courses/COURSES/FALL-2019/CS197/project/DeText/trainingSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B62DE644-573C-D541-AC42-E9F1FE1CA00B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4788B8B-1F81-C848-81A0-93CF3ACCA375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4580" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Explicit" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:Z1385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Tokenized words for implicit word search, removed punctuation, added phrases to explicit list
</commit_message>
<xml_diff>
--- a/trainingSets/explicit.xlsx
+++ b/trainingSets/explicit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manukastratta/Box Sync/STANFORD/courses/COURSES/FALL-2019/CS197/GITHUB/DeText/trainingSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manukastratta/Box Sync/STANFORD/courses/COURSES/FALL-2019/CS197/project/DeText/trainingSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CED302-B624-E840-9902-071E0B73E480}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70598AC-FB99-E742-AE81-A89C78159F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Explicit" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>date rape</t>
   </si>
@@ -61,9 +61,6 @@
     <t>pedophile</t>
   </si>
   <si>
-    <t>sexual</t>
-  </si>
-  <si>
     <t>raping</t>
   </si>
   <si>
@@ -78,12 +75,30 @@
   <si>
     <t>sexual assault</t>
   </si>
+  <si>
+    <t>forcible intercourse</t>
+  </si>
+  <si>
+    <t>sex crime</t>
+  </si>
+  <si>
+    <t>unlawful sexual intercourse</t>
+  </si>
+  <si>
+    <t>sexual abuse</t>
+  </si>
+  <si>
+    <t>sexual offense</t>
+  </si>
+  <si>
+    <t>statutory offense</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,40 +109,53 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF24292E"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF24292E"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +166,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -153,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -175,6 +209,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,7 +432,7 @@
   <dimension ref="A1:Z1385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -406,8 +442,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
+      <c r="A1" s="16" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -434,8 +470,8 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="14" t="s">
-        <v>2</v>
+      <c r="A2" s="16" t="s">
+        <v>3</v>
       </c>
       <c r="D2" s="5"/>
       <c r="G2" s="6"/>
@@ -461,7 +497,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="6"/>
@@ -488,7 +524,7 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -515,8 +551,8 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="14" t="s">
-        <v>9</v>
+      <c r="A5" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="6"/>
@@ -545,7 +581,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="6"/>
@@ -574,7 +610,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="6"/>
@@ -603,7 +639,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="6"/>
@@ -661,7 +697,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="6"/>
@@ -690,7 +726,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="6"/>
@@ -719,7 +755,7 @@
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="14" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C12" s="8"/>
       <c r="D12" s="6"/>
@@ -748,7 +784,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="6"/>
@@ -777,7 +813,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="6"/>
@@ -806,7 +842,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="6"/>
@@ -835,7 +871,7 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="6"/>
@@ -864,7 +900,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="6"/>
@@ -893,7 +929,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="6"/>
@@ -922,7 +958,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="6"/>
@@ -951,7 +987,7 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="14" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
@@ -979,8 +1015,8 @@
       <c r="Z20" s="6"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
-        <v>18</v>
+      <c r="A21" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="6"/>
@@ -1008,6 +1044,9 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="15" t="s">
+        <v>21</v>
+      </c>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -1034,6 +1073,9 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
       <c r="B23" s="4"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -1060,6 +1102,9 @@
       <c r="Z23" s="6"/>
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="15" t="s">
+        <v>22</v>
+      </c>
       <c r="B24" s="4"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1086,6 +1131,9 @@
       <c r="Z24" s="6"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="15" t="s">
+        <v>23</v>
+      </c>
       <c r="B25" s="4"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
@@ -1112,6 +1160,9 @@
       <c r="Z25" s="6"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="6"/>
@@ -39183,6 +39234,9 @@
       <c r="Z1385" s="6"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A1385">
+    <sortCondition ref="A1:A1385"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>